<commit_message>
Data Uploaded, PQ Created, Visualization Created
</commit_message>
<xml_diff>
--- a/Capstone Project/1 Combined/Dataset_YearModReg.xlsx
+++ b/Capstone Project/1 Combined/Dataset_YearModReg.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/83c531bc5c99d44a/OPMT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexd\OneDrive\Documents\GitHub\Capstone-Project-Data-Modeling-and-PowerBI\Capstone Project\1 Combined\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="13_ncr:1_{11C6B721-8C73-4110-945E-9442031AB6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2493244A-AA80-4684-93C2-16792F1B33AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFFC77E-C44D-4AB7-867E-9528C6C72405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="982" activeTab="3" xr2:uid="{6022C8B0-593D-4F6F-A13C-C62463C04408}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="982" activeTab="2" xr2:uid="{6022C8B0-593D-4F6F-A13C-C62463C04408}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelID" sheetId="15" r:id="rId1"/>
@@ -5579,52 +5579,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8651A32-43D2-43D8-B3CF-A0FDEEDC794A}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>2015</v>
-      </c>
-      <c r="C2">
-        <v>2016</v>
-      </c>
-      <c r="D2">
-        <v>2017</v>
-      </c>
-      <c r="E2">
-        <v>2018</v>
-      </c>
-      <c r="F2">
-        <v>2019</v>
+      <c r="B6">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>
@@ -5636,7 +5644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB33C8B5-5F73-459C-9C11-58E251AB09B1}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>